<commit_message>
Intigration Of Similarity score feature in Main
</commit_message>
<xml_diff>
--- a/data/similarity_score.xlsx
+++ b/data/similarity_score.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,99 +436,666 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>1_.txt</t>
+          <t>assignment_CTV10_text.txt</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>2_.txt</t>
+          <t>assignment_CTV11_text.txt</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>3_.txt</t>
+          <t>assignment_CTV12_text.txt</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>IMG_20240724_221056_text.txt</t>
+          <t>assignment_CTV13_text.txt</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV1_text.txt</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV2_text.txt</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV3_text.txt</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV4_text.txt</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV5_text.txt</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV6_text.txt</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV7_text.txt</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV8_text.txt</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV9_text.txt</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>1_.txt</t>
+          <t>assignment_CTV10_text.txt</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9999999999999996</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9922887654931783</v>
+        <v>0.4909059523616331</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9892784660394022</v>
+        <v>0.4730416612393216</v>
       </c>
       <c r="E2" t="n">
-        <v>0.988715620394053</v>
+        <v>0.3621270807762046</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.2129800892548739</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.4570185002308301</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.4529824681661435</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.3050798131998193</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.3236211480533297</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.4649663225577514</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.3175445631164253</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.2638463710426938</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.2525280048869465</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2_.txt</t>
+          <t>assignment_CTV11_text.txt</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9922887654931783</v>
+        <v>0.4909059523616331</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9999999999999996</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9899569275557604</v>
+        <v>0.4505100514162388</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9894446830276915</v>
+        <v>0.3248213843027175</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.1838168531564767</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.5626847746084883</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.4985644000420552</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.3670293827061656</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.3181533344857441</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.5061407192242275</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.4005880815941841</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.2929338374249789</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.2821595945597417</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>3_.txt</t>
+          <t>assignment_CTV12_text.txt</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9892784660394022</v>
+        <v>0.4730416612393216</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9899569275557604</v>
+        <v>0.4505100514162388</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9891794182206929</v>
+        <v>0.3790243344199932</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.2059238145267305</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.4438244286916023</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.4890065770352529</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.3777450768035944</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.3392493682923026</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.4323355761034904</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.3955729725457514</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.3555315693617424</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.3201327258403701</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>IMG_20240724_221056_text.txt</t>
+          <t>assignment_CTV13_text.txt</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.988715620394053</v>
+        <v>0.3621270807762046</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9894446830276915</v>
+        <v>0.3248213843027175</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9891794182206929</v>
+        <v>0.3790243344199932</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.2195177405121774</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.3473335394526259</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.4399667560683506</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.2080097337779624</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.2939930495271302</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.3734217090715743</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.3929509726116982</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.2668881083243967</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.3461960494203722</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV1_text.txt</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.2129800892548739</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1838168531564767</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2059238145267305</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.2195177405121774</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.2210669991438392</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.1901868796089854</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.1599519164327813</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.1977204279822128</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.1942182726475837</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.2251984521895539</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.2056263806357369</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.2379460401762244</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV2_text.txt</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.4570185002308301</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.5626847746084883</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.4438244286916023</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.3473335394526259</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.2210669991438392</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.5390812417710448</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.3809818784815964</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.3380840551841366</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.5241746377226013</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.398445839470171</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.3091303029943553</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.3271514040437998</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV3_text.txt</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.4529824681661435</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.4985644000420552</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.4890065770352529</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.4399667560683506</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1901868796089854</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.5390812417710448</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.9999999999999997</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.3544770862868643</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.3373142884687338</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.5307927402048629</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.4660558857748328</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.4306522625336323</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.3759109978148535</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV4_text.txt</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.3050798131998193</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.3670293827061656</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3777450768035944</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.2080097337779624</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.1599519164327813</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.3809818784815964</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.3544770862868643</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.2469693319741462</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.3916603562779996</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.2972771513124131</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.3221740039722897</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.2237012068197454</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV5_text.txt</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.3236211480533297</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.3181533344857441</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.3392493682923026</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.2939930495271302</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.1977204279822128</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.3380840551841366</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.3373142884687338</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.2469693319741462</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.3292731669097152</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.34147894282933</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.2431741788976065</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.2407336358517829</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV6_text.txt</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.4649663225577514</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.5061407192242275</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.4323355761034904</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.3734217090715743</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.1942182726475837</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.5241746377226013</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.5307927402048629</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.3916603562779996</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.3292731669097152</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1.000000000000003</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.4121639833873383</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.3293408174105021</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.3162451044774767</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV7_text.txt</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.3175445631164253</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.4005880815941841</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.3955729725457514</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.3929509726116982</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.2251984521895539</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.398445839470171</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.4660558857748328</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.2972771513124131</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.34147894282933</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.4121639833873383</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.3892225350205452</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.429932136706347</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV8_text.txt</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.2638463710426938</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.2929338374249789</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.3555315693617424</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.2668881083243967</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.2056263806357369</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.3091303029943553</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.4306522625336323</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.3221740039722897</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.2431741788976065</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.3293408174105021</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.3892225350205452</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.4119736214363552</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>assignment_CTV9_text.txt</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.2525280048869465</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.2821595945597417</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.3201327258403701</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.3461960494203722</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.2379460401762244</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.3271514040437998</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.3759109978148535</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.2237012068197454</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.2407336358517829</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.3162451044774767</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.429932136706347</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.4119736214363552</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.9999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>